<commit_message>
updating model runs and adding data for MIS4
</commit_message>
<xml_diff>
--- a/cost-rasters/input-data/lakes/lake-levels.xlsx
+++ b/cost-rasters/input-data/lakes/lake-levels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilycoco/Desktop/ab-lcp-dispersals/cost-rasters/input-data/lakes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20CAD6A-5957-4F47-BE91-621443D7EA80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C647479-F759-1845-B0C6-79D3D6CD8E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{9550B7EE-BCEB-9E4F-ADE2-5BAC506EF63A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16200" xr2:uid="{9550B7EE-BCEB-9E4F-ADE2-5BAC506EF63A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="82">
   <si>
     <t>Level m asl</t>
   </si>
@@ -116,9 +116,6 @@
     <t>MIS 5</t>
   </si>
   <si>
-    <t>Korsakova 2009</t>
-  </si>
-  <si>
     <t>Black Sea</t>
   </si>
   <si>
@@ -155,9 +152,6 @@
     <t>70-90 ka</t>
   </si>
   <si>
-    <t>late MIS 5</t>
-  </si>
-  <si>
     <t>Ob River</t>
   </si>
   <si>
@@ -173,18 +167,12 @@
     <t>Astakhov 2006</t>
   </si>
   <si>
-    <t>Lake Komi</t>
-  </si>
-  <si>
     <t>Kurbanov et al 2021; Dolukhanov et al 2010</t>
   </si>
   <si>
     <t>Citations</t>
   </si>
   <si>
-    <t>Astakhov 2006; Komatsu et al 2016</t>
-  </si>
-  <si>
     <t>Manych Pass (Caspian, Black)</t>
   </si>
   <si>
@@ -221,18 +209,12 @@
     <t>Mangerund 2004; Mangerund et al 2001</t>
   </si>
   <si>
-    <t>Lake flooding notes -- try flooding rivers with glaciers in place</t>
-  </si>
-  <si>
     <t>DONE</t>
   </si>
   <si>
     <t>YES</t>
   </si>
   <si>
-    <t>YES (Barents)</t>
-  </si>
-  <si>
     <t>Dnieper River</t>
   </si>
   <si>
@@ -252,6 +234,54 @@
   </si>
   <si>
     <t>Svitoch 2009</t>
+  </si>
+  <si>
+    <t>MIS 5a</t>
+  </si>
+  <si>
+    <t>MIS 5b</t>
+  </si>
+  <si>
+    <t>MIS 5c</t>
+  </si>
+  <si>
+    <t>MIS 5d</t>
+  </si>
+  <si>
+    <t>MIS 5e</t>
+  </si>
+  <si>
+    <t>Dalton et al 2021</t>
+  </si>
+  <si>
+    <t>MIS 4/3</t>
+  </si>
+  <si>
+    <t>Kurbanov et al 2021; Dolukhanov et al 2010; Bezrodnykh et al 2020</t>
+  </si>
+  <si>
+    <t>Költringer et al 2020</t>
+  </si>
+  <si>
+    <t>late MIS 5 (MIS 5b)</t>
+  </si>
+  <si>
+    <t>NOTES</t>
+  </si>
+  <si>
+    <t>When sea levels are unknown, levels from closest similar period are used</t>
+  </si>
+  <si>
+    <t>Korsakova 2009; Astakhov 2006; Komatsu et al 2016</t>
+  </si>
+  <si>
+    <t>0 to 10</t>
+  </si>
+  <si>
+    <t>MIS 5a-d</t>
+  </si>
+  <si>
+    <t>Late Khazarian (Eemian)</t>
   </si>
 </sst>
 </file>
@@ -630,23 +660,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D06732-6BD1-EF41-82D4-0268B7334728}">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -661,53 +691,59 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B2" s="5">
         <v>57</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="4">
         <v>60</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="4">
         <v>140</v>
@@ -715,16 +751,13 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="I4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -745,7 +778,7 @@
         <v>7</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -763,10 +796,10 @@
         <v>17</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -784,10 +817,10 @@
         <v>17</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -807,67 +840,67 @@
         <v>17</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>68</v>
+      <c r="F9" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10">
-        <v>-140</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" t="s">
-        <v>4</v>
+        <v>26</v>
+      </c>
+      <c r="B10" s="2">
+        <v>-25</v>
       </c>
       <c r="E10" t="s">
         <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="G10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="2">
-        <v>-25</v>
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>-140</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="F11" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="G11" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -884,395 +917,513 @@
         <v>23</v>
       </c>
       <c r="G12" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B13" s="2">
         <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E13" t="s">
         <v>22</v>
       </c>
       <c r="F13" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G13" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E14" t="s">
         <v>22</v>
       </c>
       <c r="F14" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G14" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15">
         <v>45</v>
       </c>
       <c r="D15" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E15" t="s">
         <v>22</v>
       </c>
       <c r="F15" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G15" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B16" s="3">
         <v>80</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
         <v>22</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B17">
-        <v>90</v>
-      </c>
-      <c r="D17" t="s">
-        <v>41</v>
+        <v>-30</v>
       </c>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="F17" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="G17" t="s">
-        <v>63</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18">
+        <v>12</v>
+      </c>
+      <c r="E18" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" t="s">
+        <v>71</v>
+      </c>
+      <c r="G18" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="2">
-        <v>70</v>
-      </c>
-      <c r="C19" t="s">
         <v>38</v>
       </c>
+      <c r="B19">
+        <v>90</v>
+      </c>
+      <c r="D19" t="s">
+        <v>39</v>
+      </c>
       <c r="E19" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="F19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G19" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="B20">
-        <v>100</v>
-      </c>
-      <c r="D20" t="s">
-        <v>24</v>
+        <v>70</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
       </c>
       <c r="E20" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="F20" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G20" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="2">
-        <v>60</v>
-      </c>
-      <c r="D21" t="s">
-        <v>42</v>
+        <v>30</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="F21" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="G21" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="2">
-        <v>70</v>
+        <v>45</v>
+      </c>
+      <c r="B22">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
+        <v>46</v>
       </c>
       <c r="D22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E22" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="F22" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G22" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="2">
-        <v>100</v>
+        <v>52</v>
+      </c>
+      <c r="B23">
+        <v>126</v>
+      </c>
+      <c r="C23" t="s">
+        <v>46</v>
       </c>
       <c r="D23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E23" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="F23" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="G23" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" s="2">
-        <v>26</v>
+        <v>48</v>
+      </c>
+      <c r="B24">
+        <v>57</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E24" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="F24" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G24" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>56</v>
-      </c>
-      <c r="B25" s="2">
-        <v>126</v>
-      </c>
-      <c r="C25" t="s">
-        <v>50</v>
-      </c>
-      <c r="D25" t="s">
-        <v>42</v>
+        <v>30</v>
+      </c>
+      <c r="B25">
+        <v>-25</v>
       </c>
       <c r="E25" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="F25" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G25" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" s="2">
-        <v>57</v>
-      </c>
-      <c r="C26" t="s">
-        <v>50</v>
-      </c>
-      <c r="D26" t="s">
-        <v>42</v>
+        <v>30</v>
+      </c>
+      <c r="B26">
+        <v>-60</v>
       </c>
       <c r="E26" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="F26" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G26" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B27" s="3">
-        <v>140</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>66</v>
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27">
+        <v>-60</v>
+      </c>
+      <c r="E27" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" t="s">
+        <v>62</v>
+      </c>
+      <c r="G27" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="2">
-        <v>135</v>
+        <v>21</v>
+      </c>
+      <c r="B28">
+        <v>100</v>
+      </c>
+      <c r="D28" t="s">
+        <v>24</v>
       </c>
       <c r="E28" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="F28" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="G28" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29">
-        <v>10</v>
-      </c>
-      <c r="D29" t="s">
-        <v>14</v>
+        <v>30</v>
+      </c>
+      <c r="B29" t="s">
+        <v>79</v>
       </c>
       <c r="E29" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="F29" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="G29" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>27</v>
-      </c>
-      <c r="B30" s="2">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="B30">
+        <v>-5</v>
       </c>
       <c r="D30" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="E30" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="F30" t="s">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="G30" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B31">
         <v>60</v>
       </c>
       <c r="D31" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E31" t="s">
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="F31" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="G31" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>31</v>
-      </c>
-      <c r="B32" s="2">
+        <v>41</v>
+      </c>
+      <c r="B32">
+        <v>70</v>
+      </c>
+      <c r="D32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32" t="s">
+        <v>80</v>
+      </c>
+      <c r="F32" t="s">
+        <v>42</v>
+      </c>
+      <c r="G32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" s="3">
+        <v>140</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34">
+        <v>135</v>
+      </c>
+      <c r="E34" t="s">
+        <v>35</v>
+      </c>
+      <c r="F34" t="s">
+        <v>29</v>
+      </c>
+      <c r="G34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35">
+        <v>10</v>
+      </c>
+      <c r="D35" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" t="s">
+        <v>18</v>
+      </c>
+      <c r="G35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="2">
+        <v>6</v>
+      </c>
+      <c r="D36" t="s">
+        <v>27</v>
+      </c>
+      <c r="E36" t="s">
+        <v>19</v>
+      </c>
+      <c r="F36" t="s">
+        <v>28</v>
+      </c>
+      <c r="G36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37">
+        <v>60</v>
+      </c>
+      <c r="D37" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" t="s">
+        <v>23</v>
+      </c>
+      <c r="G37" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="2">
         <v>120</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E38" t="s">
         <v>15</v>
       </c>
-      <c r="F32" t="s">
-        <v>30</v>
-      </c>
-      <c r="G32" t="s">
-        <v>63</v>
+      <c r="F38" t="s">
+        <v>29</v>
+      </c>
+      <c r="G38" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>